<commit_message>
Added 125 g/L (25 and 50% recovery) for COMRO and OARO
</commit_message>
<xml_diff>
--- a/DesalinationModels/EnhancedRO_APM_Models/model_summary_variable_description.xlsx
+++ b/DesalinationModels/EnhancedRO_APM_Models/model_summary_variable_description.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adama\DOE_CSP_PROJECT\DesalinationModels\EnhancedRO_APM_Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11CE874B-2545-4F72-A979-EE09ED1DE469}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3ED3C02-0071-43D6-992B-6BC2284E1710}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="2" xr2:uid="{CF93556C-6F60-4EE5-8404-2CC0F06205D7}"/>
   </bookViews>
@@ -238,14 +238,14 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -565,7 +565,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -587,10 +587,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -611,10 +611,10 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C5" t="s">
@@ -622,10 +622,10 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C6" t="s">
@@ -698,23 +698,23 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="5" t="s">
         <v>47</v>
       </c>
     </row>
@@ -728,7 +728,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBEA58EC-4FC3-4F57-A504-E1DF4203F112}">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
@@ -740,11 +740,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
@@ -758,10 +758,10 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -782,18 +782,18 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -863,28 +863,28 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="17" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
@@ -898,10 +898,10 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -922,10 +922,10 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C23" t="s">
@@ -933,10 +933,10 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1006,18 +1006,18 @@
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="2" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1036,13 +1036,13 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="28.73046875" customWidth="1"/>
-    <col min="2" max="2" width="21.59765625" customWidth="1"/>
+    <col min="2" max="2" width="26.46484375" customWidth="1"/>
     <col min="3" max="3" width="20.265625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1058,10 +1058,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1082,10 +1082,10 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C5" t="s">
@@ -1093,10 +1093,10 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1166,23 +1166,23 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>